<commit_message>
Operacion MODULO y actualizacion de matriz para determinar el tipo de dato resultante para la misma operacion
</commit_message>
<xml_diff>
--- a/Proyecto1/matrizTipoDato.xlsx
+++ b/Proyecto1/matrizTipoDato.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlzdr\OneDrive\Escritorio\COMPILADORES\OLC2Proyecto1\OLC2Proyecto1\Proyecto1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlzdr\OneDrive\Documentos\OLC2Proyecto2\OLC2Proyecto2_201314821\Proyecto1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC913699-1A4F-454C-A996-AA27F3BCC8C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346A0D58-9A9E-4873-9732-2BBB578429F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-945" windowWidth="19440" windowHeight="14880" xr2:uid="{927AAAB6-833E-418D-BC07-C7F753115376}"/>
   </bookViews>
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76B28D81-03FD-490F-86D3-FE47E2376840}">
   <dimension ref="A3:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45:H49"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,14 +1168,14 @@
         <v>4</v>
       </c>
       <c r="F37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37" t="s">
         <v>4</v>
       </c>
       <c r="H37" t="str">
         <f>CONCATENATE("{",C37,",",D37,",",E37,",",F37,",",G37,"},")</f>
-        <v>{INTEGER,NULO,NULO,FLOAT,NULO},</v>
+        <v>{INTEGER,NULO,NULO,INTEGER,NULO},</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>